<commit_message>
CCRU POS update + script
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/Canteen PoS 2018.xlsx
+++ b/Projects/CCRU/Data/Canteen PoS 2018.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Canteen" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,6 +28,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Canteen!$A$1:$AQ$41</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Canteen!$A$1:$AQ$41</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Canteen!$A$1:$AQ$41</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Canteen!$A$1:$AQ$41</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="205">
   <si>
     <t xml:space="preserve">Sorting</t>
   </si>
@@ -387,16 +388,28 @@
     <t xml:space="preserve">Добрый - Апельсин - 0.33л</t>
   </si>
   <si>
-    <t xml:space="preserve">Moya Semya - Apple - 0.2L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Моя Семья - Яблоко - 0.2л</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moya Semya - Multifruit - 0.2L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Моя Семья - Мультифрут - 0.2л</t>
+    <t xml:space="preserve">Moya Semya - Apple mix - 0.175L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Моя Семья - Яблочный Микс - 0.175л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moya Semya - Apple mix - 0.175L, Moya Semya - Apple - 0.2L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4650075421192, 4607174578265</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moya Semya - Multifruit - 0.175L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Моя Семья - Мульти-Фрути - 0.175л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moya Semya - Multifruit - 0.175L, Moya Semya - Multifruit - 0.2L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4650075421338, 4607174578586</t>
   </si>
   <si>
     <t xml:space="preserve">Dobriy - Peach-Apple - 0.33L</t>
@@ -758,7 +771,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -769,6 +782,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
     <fill>
@@ -838,7 +857,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="38">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -919,6 +938,22 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -959,7 +994,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1062,14 +1097,14 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+      <selection pane="bottomLeft" activeCell="L25" activeCellId="0" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="32.45"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="1" width="15.246963562753"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="42.4493927125506"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="15.246963562753"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="1" width="15.5465587044534"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="43.4615384615385"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="15.5465587044534"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="62.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3271,10 +3306,10 @@
         <v>73</v>
       </c>
       <c r="F26" s="8"/>
-      <c r="G26" s="13" t="s">
+      <c r="G26" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="H26" s="13" t="s">
+      <c r="H26" s="20" t="s">
         <v>110</v>
       </c>
       <c r="I26" s="8" t="s">
@@ -3286,11 +3321,11 @@
       </c>
       <c r="L26" s="8"/>
       <c r="M26" s="8"/>
-      <c r="N26" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="O26" s="9" t="n">
-        <v>4607174578265</v>
+      <c r="N26" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="O26" s="22" t="s">
+        <v>112</v>
       </c>
       <c r="P26" s="8"/>
       <c r="Q26" s="8"/>
@@ -3359,11 +3394,11 @@
         <v>73</v>
       </c>
       <c r="F27" s="8"/>
-      <c r="G27" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="H27" s="13" t="s">
-        <v>112</v>
+      <c r="G27" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="H27" s="20" t="s">
+        <v>114</v>
       </c>
       <c r="I27" s="8" t="s">
         <v>55</v>
@@ -3374,11 +3409,11 @@
       </c>
       <c r="L27" s="8"/>
       <c r="M27" s="8"/>
-      <c r="N27" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="O27" s="9" t="n">
-        <v>4607174578586</v>
+      <c r="N27" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="O27" s="22" t="s">
+        <v>116</v>
       </c>
       <c r="P27" s="8"/>
       <c r="Q27" s="8"/>
@@ -3448,10 +3483,10 @@
       </c>
       <c r="F28" s="8"/>
       <c r="G28" s="11" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="H28" s="13" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="I28" s="8" t="s">
         <v>55</v>
@@ -3463,7 +3498,7 @@
       <c r="L28" s="8"/>
       <c r="M28" s="8"/>
       <c r="N28" s="8" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="O28" s="9" t="n">
         <v>4607174579262</v>
@@ -3532,17 +3567,17 @@
         <v>46</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="7" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="J29" s="0"/>
       <c r="K29" s="7" t="n">
@@ -3552,7 +3587,7 @@
       <c r="M29" s="7"/>
       <c r="N29" s="7"/>
       <c r="O29" s="11" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="P29" s="7"/>
       <c r="Q29" s="7"/>
@@ -3560,7 +3595,7 @@
         <v>56</v>
       </c>
       <c r="S29" s="7" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="T29" s="7"/>
       <c r="U29" s="7"/>
@@ -3568,7 +3603,7 @@
       <c r="W29" s="7"/>
       <c r="X29" s="7"/>
       <c r="Y29" s="11" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="Z29" s="7"/>
       <c r="AA29" s="7"/>
@@ -3580,7 +3615,7 @@
       <c r="AE29" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="AF29" s="20" t="n">
+      <c r="AF29" s="24" t="n">
         <v>0.1</v>
       </c>
       <c r="AG29" s="7"/>
@@ -3616,14 +3651,14 @@
         <v>46</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="F30" s="7"/>
       <c r="G30" s="7" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="I30" s="7" t="s">
         <v>55</v>
@@ -3635,32 +3670,32 @@
       <c r="L30" s="7"/>
       <c r="M30" s="7"/>
       <c r="N30" s="7" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="O30" s="7" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="P30" s="7" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="Q30" s="7"/>
       <c r="R30" s="7" t="s">
         <v>56</v>
       </c>
       <c r="S30" s="7" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="T30" s="7" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="U30" s="7"/>
       <c r="V30" s="7"/>
       <c r="W30" s="7"/>
       <c r="X30" s="7" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="Y30" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="Z30" s="7"/>
       <c r="AA30" s="7"/>
@@ -3672,7 +3707,7 @@
       <c r="AE30" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="AF30" s="20" t="n">
+      <c r="AF30" s="24" t="n">
         <v>0.1</v>
       </c>
       <c r="AG30" s="7"/>
@@ -3708,14 +3743,14 @@
         <v>46</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="7" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="I31" s="7" t="s">
         <v>55</v>
@@ -3727,32 +3762,32 @@
       <c r="L31" s="7"/>
       <c r="M31" s="7"/>
       <c r="N31" s="7" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="O31" s="8" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="P31" s="8" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="Q31" s="7"/>
       <c r="R31" s="7" t="s">
         <v>56</v>
       </c>
       <c r="S31" s="7" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="T31" s="7" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="U31" s="7"/>
       <c r="V31" s="7"/>
       <c r="W31" s="7"/>
       <c r="X31" s="7" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="Y31" s="7" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="Z31" s="7"/>
       <c r="AA31" s="7"/>
@@ -3764,7 +3799,7 @@
       <c r="AE31" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="AF31" s="20" t="n">
+      <c r="AF31" s="24" t="n">
         <v>0.1</v>
       </c>
       <c r="AG31" s="7"/>
@@ -3800,28 +3835,28 @@
         <v>46</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="F32" s="7"/>
       <c r="G32" s="8" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="J32" s="8"/>
       <c r="K32" s="0"/>
       <c r="L32" s="8"/>
       <c r="M32" s="8"/>
       <c r="N32" s="7"/>
-      <c r="O32" s="21"/>
-      <c r="P32" s="21"/>
-      <c r="Q32" s="21"/>
+      <c r="O32" s="25"/>
+      <c r="P32" s="25"/>
+      <c r="Q32" s="25"/>
       <c r="R32" s="7" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="S32" s="7"/>
       <c r="T32" s="7"/>
@@ -3838,7 +3873,7 @@
         <v>51</v>
       </c>
       <c r="AE32" s="8" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="AF32" s="15" t="n">
         <v>0.08</v>
@@ -3846,7 +3881,7 @@
       <c r="AG32" s="8"/>
       <c r="AH32" s="8"/>
       <c r="AI32" s="8" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="AJ32" s="8"/>
       <c r="AK32" s="8"/>
@@ -3858,7 +3893,7 @@
         <v>31</v>
       </c>
       <c r="AO32" s="10" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="AP32" s="7"/>
       <c r="AQ32" s="7"/>
@@ -3878,17 +3913,17 @@
         <v>46</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="F33" s="7"/>
       <c r="G33" s="8" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="I33" s="8" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="J33" s="8"/>
       <c r="K33" s="8" t="n">
@@ -3897,7 +3932,7 @@
       <c r="L33" s="8"/>
       <c r="M33" s="8"/>
       <c r="N33" s="7" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="O33" s="9"/>
       <c r="P33" s="9"/>
@@ -3909,7 +3944,7 @@
       <c r="V33" s="7"/>
       <c r="W33" s="7"/>
       <c r="X33" s="8" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="Y33" s="7"/>
       <c r="Z33" s="7"/>
@@ -3928,7 +3963,7 @@
       <c r="AG33" s="8"/>
       <c r="AH33" s="8"/>
       <c r="AI33" s="8" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="AJ33" s="8"/>
       <c r="AK33" s="8"/>
@@ -3941,7 +3976,7 @@
       </c>
       <c r="AO33" s="7"/>
       <c r="AP33" s="7" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="AQ33" s="7"/>
       <c r="AR33" s="12"/>
@@ -3960,17 +3995,17 @@
         <v>46</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="F34" s="7"/>
       <c r="G34" s="8" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="I34" s="8" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="J34" s="8"/>
       <c r="K34" s="8" t="n">
@@ -3979,21 +4014,21 @@
       <c r="L34" s="8"/>
       <c r="M34" s="8"/>
       <c r="N34" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="O34" s="21"/>
-      <c r="P34" s="21"/>
-      <c r="Q34" s="21"/>
+        <v>148</v>
+      </c>
+      <c r="O34" s="25"/>
+      <c r="P34" s="25"/>
+      <c r="Q34" s="25"/>
       <c r="R34" s="7"/>
       <c r="S34" s="7" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="T34" s="7"/>
       <c r="U34" s="7"/>
       <c r="V34" s="7"/>
       <c r="W34" s="7"/>
       <c r="X34" s="8" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="Y34" s="7"/>
       <c r="Z34" s="7"/>
@@ -4023,7 +4058,7 @@
       </c>
       <c r="AO34" s="7"/>
       <c r="AP34" s="7" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="AQ34" s="7"/>
       <c r="AR34" s="12"/>
@@ -4042,17 +4077,17 @@
         <v>46</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="F35" s="7"/>
       <c r="G35" s="8" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="H35" s="11" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="J35" s="0"/>
       <c r="K35" s="11" t="n">
@@ -4062,25 +4097,25 @@
       <c r="M35" s="8"/>
       <c r="N35" s="7"/>
       <c r="O35" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="P35" s="21"/>
-      <c r="Q35" s="21"/>
+        <v>159</v>
+      </c>
+      <c r="P35" s="25"/>
+      <c r="Q35" s="25"/>
       <c r="R35" s="7"/>
       <c r="S35" s="7" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="T35" s="7"/>
       <c r="U35" s="7"/>
-      <c r="V35" s="22"/>
+      <c r="V35" s="26"/>
       <c r="W35" s="7"/>
       <c r="X35" s="8" t="s">
         <v>58</v>
       </c>
       <c r="Y35" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="Z35" s="22"/>
+        <v>159</v>
+      </c>
+      <c r="Z35" s="26"/>
       <c r="AA35" s="8"/>
       <c r="AB35" s="7"/>
       <c r="AC35" s="7"/>
@@ -4096,12 +4131,12 @@
       <c r="AG35" s="8"/>
       <c r="AH35" s="8"/>
       <c r="AI35" s="8" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="AJ35" s="8"/>
       <c r="AK35" s="8"/>
       <c r="AL35" s="8" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="AM35" s="7" t="n">
         <v>2</v>
@@ -4110,8 +4145,8 @@
         <v>34</v>
       </c>
       <c r="AO35" s="7"/>
-      <c r="AP35" s="23" t="s">
-        <v>157</v>
+      <c r="AP35" s="27" t="s">
+        <v>161</v>
       </c>
       <c r="AQ35" s="7"/>
       <c r="AR35" s="12"/>
@@ -4130,17 +4165,17 @@
         <v>46</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="F36" s="7"/>
       <c r="G36" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="H36" s="24" t="s">
-        <v>159</v>
+        <v>162</v>
+      </c>
+      <c r="H36" s="28" t="s">
+        <v>163</v>
       </c>
       <c r="I36" s="11" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="J36" s="11"/>
       <c r="K36" s="8" t="n">
@@ -4149,21 +4184,21 @@
       <c r="L36" s="8"/>
       <c r="M36" s="8"/>
       <c r="N36" s="7" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="O36" s="9"/>
       <c r="P36" s="9"/>
       <c r="Q36" s="9"/>
       <c r="R36" s="7"/>
       <c r="S36" s="7" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="T36" s="8"/>
       <c r="U36" s="8"/>
       <c r="V36" s="7"/>
       <c r="W36" s="7"/>
       <c r="X36" s="8" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="Y36" s="8"/>
       <c r="Z36" s="7"/>
@@ -4174,7 +4209,7 @@
         <v>51</v>
       </c>
       <c r="AE36" s="8" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="AF36" s="15" t="n">
         <v>0.04</v>
@@ -4182,12 +4217,12 @@
       <c r="AG36" s="8"/>
       <c r="AH36" s="8"/>
       <c r="AI36" s="8" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="AJ36" s="8"/>
       <c r="AK36" s="8"/>
       <c r="AL36" s="8" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="AM36" s="7" t="n">
         <v>2</v>
@@ -4196,8 +4231,8 @@
         <v>35</v>
       </c>
       <c r="AO36" s="7"/>
-      <c r="AP36" s="23" t="s">
-        <v>157</v>
+      <c r="AP36" s="27" t="s">
+        <v>161</v>
       </c>
       <c r="AQ36" s="7"/>
       <c r="AR36" s="12"/>
@@ -4216,17 +4251,17 @@
         <v>46</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="F37" s="7"/>
       <c r="G37" s="8" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="I37" s="11" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="J37" s="11"/>
       <c r="K37" s="8"/>
@@ -4237,11 +4272,11 @@
         <v>19</v>
       </c>
       <c r="N37" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="O37" s="21"/>
-      <c r="P37" s="21"/>
-      <c r="Q37" s="21"/>
+        <v>148</v>
+      </c>
+      <c r="O37" s="25"/>
+      <c r="P37" s="25"/>
+      <c r="Q37" s="25"/>
       <c r="R37" s="7"/>
       <c r="S37" s="7"/>
       <c r="T37" s="7"/>
@@ -4249,7 +4284,7 @@
       <c r="V37" s="7"/>
       <c r="W37" s="7"/>
       <c r="X37" s="8" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="Y37" s="7"/>
       <c r="Z37" s="7"/>
@@ -4260,7 +4295,7 @@
         <v>51</v>
       </c>
       <c r="AE37" s="8" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="AF37" s="15" t="n">
         <v>0.04</v>
@@ -4268,12 +4303,12 @@
       <c r="AG37" s="8"/>
       <c r="AH37" s="8"/>
       <c r="AI37" s="8" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="AJ37" s="8"/>
       <c r="AK37" s="8"/>
       <c r="AL37" s="8" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="AM37" s="7" t="n">
         <v>2</v>
@@ -4282,8 +4317,8 @@
         <v>36</v>
       </c>
       <c r="AO37" s="7"/>
-      <c r="AP37" s="23" t="s">
-        <v>157</v>
+      <c r="AP37" s="27" t="s">
+        <v>161</v>
       </c>
       <c r="AQ37" s="7"/>
       <c r="AR37" s="12"/>
@@ -4302,17 +4337,17 @@
         <v>46</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="F38" s="7"/>
       <c r="G38" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="H38" s="25" t="s">
-        <v>167</v>
+        <v>170</v>
+      </c>
+      <c r="H38" s="29" t="s">
+        <v>171</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="J38" s="8"/>
       <c r="K38" s="7" t="n">
@@ -4325,7 +4360,7 @@
       <c r="P38" s="7"/>
       <c r="Q38" s="7"/>
       <c r="R38" s="7" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="S38" s="7"/>
       <c r="T38" s="7"/>
@@ -4333,10 +4368,10 @@
       <c r="V38" s="7"/>
       <c r="W38" s="7"/>
       <c r="X38" s="7" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="Y38" s="7" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="Z38" s="7"/>
       <c r="AA38" s="7"/>
@@ -4348,7 +4383,7 @@
       <c r="AE38" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="AF38" s="20" t="n">
+      <c r="AF38" s="24" t="n">
         <v>0.1</v>
       </c>
       <c r="AG38" s="7"/>
@@ -4364,7 +4399,7 @@
         <v>37</v>
       </c>
       <c r="AO38" s="10" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="AP38" s="7"/>
       <c r="AQ38" s="7"/>
@@ -4386,14 +4421,14 @@
         <v>46</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="F39" s="7"/>
       <c r="G39" s="7" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="I39" s="7" t="s">
         <v>55</v>
@@ -4405,10 +4440,10 @@
       <c r="L39" s="7"/>
       <c r="M39" s="7"/>
       <c r="N39" s="8" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="O39" s="8" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="P39" s="7"/>
       <c r="Q39" s="7"/>
@@ -4423,10 +4458,10 @@
       <c r="V39" s="7"/>
       <c r="W39" s="7"/>
       <c r="X39" s="7" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="Y39" s="7" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="Z39" s="7"/>
       <c r="AA39" s="7"/>
@@ -4438,7 +4473,7 @@
       <c r="AE39" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="AF39" s="20" t="n">
+      <c r="AF39" s="24" t="n">
         <v>0</v>
       </c>
       <c r="AG39" s="7"/>
@@ -4455,7 +4490,7 @@
       </c>
       <c r="AO39" s="7"/>
       <c r="AP39" s="7" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="AQ39" s="7"/>
       <c r="AR39" s="12"/>
@@ -4474,14 +4509,14 @@
         <v>46</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="F40" s="7"/>
       <c r="G40" s="7" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="I40" s="7" t="s">
         <v>55</v>
@@ -4493,7 +4528,7 @@
       <c r="L40" s="7"/>
       <c r="M40" s="7"/>
       <c r="N40" s="7" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="O40" s="7" t="n">
         <v>5000034</v>
@@ -4511,10 +4546,10 @@
       <c r="V40" s="7"/>
       <c r="W40" s="7"/>
       <c r="X40" s="7" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="Y40" s="7" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="Z40" s="7"/>
       <c r="AA40" s="7"/>
@@ -4526,13 +4561,13 @@
       <c r="AE40" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="AF40" s="20" t="n">
+      <c r="AF40" s="24" t="n">
         <v>0</v>
       </c>
       <c r="AG40" s="7"/>
       <c r="AH40" s="7"/>
       <c r="AI40" s="7" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="AJ40" s="7"/>
       <c r="AK40" s="7"/>
@@ -4545,7 +4580,7 @@
       </c>
       <c r="AO40" s="7"/>
       <c r="AP40" s="7" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="AQ40" s="7"/>
       <c r="AR40" s="12"/>
@@ -4560,66 +4595,66 @@
       <c r="C41" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D41" s="24" t="s">
-        <v>180</v>
-      </c>
-      <c r="E41" s="26" t="s">
-        <v>181</v>
-      </c>
-      <c r="F41" s="26" t="s">
-        <v>182</v>
-      </c>
-      <c r="G41" s="26" t="s">
-        <v>157</v>
-      </c>
-      <c r="H41" s="27"/>
-      <c r="I41" s="27" t="s">
-        <v>183</v>
-      </c>
-      <c r="J41" s="27" t="s">
+      <c r="D41" s="28" t="s">
         <v>184</v>
       </c>
-      <c r="K41" s="27"/>
-      <c r="L41" s="27"/>
-      <c r="M41" s="28"/>
-      <c r="N41" s="28"/>
-      <c r="O41" s="27"/>
-      <c r="P41" s="27"/>
-      <c r="Q41" s="27"/>
-      <c r="R41" s="27"/>
-      <c r="S41" s="27" t="s">
+      <c r="E41" s="30" t="s">
         <v>185</v>
       </c>
-      <c r="T41" s="27"/>
-      <c r="U41" s="27"/>
-      <c r="V41" s="27"/>
-      <c r="W41" s="27"/>
-      <c r="X41" s="27"/>
-      <c r="Y41" s="27"/>
-      <c r="Z41" s="27"/>
-      <c r="AA41" s="27"/>
-      <c r="AB41" s="27"/>
-      <c r="AC41" s="27"/>
-      <c r="AD41" s="27"/>
-      <c r="AE41" s="27"/>
-      <c r="AF41" s="29" t="n">
+      <c r="F41" s="30" t="s">
+        <v>186</v>
+      </c>
+      <c r="G41" s="30" t="s">
+        <v>161</v>
+      </c>
+      <c r="H41" s="31"/>
+      <c r="I41" s="31" t="s">
+        <v>187</v>
+      </c>
+      <c r="J41" s="31" t="s">
+        <v>188</v>
+      </c>
+      <c r="K41" s="31"/>
+      <c r="L41" s="31"/>
+      <c r="M41" s="32"/>
+      <c r="N41" s="32"/>
+      <c r="O41" s="31"/>
+      <c r="P41" s="31"/>
+      <c r="Q41" s="31"/>
+      <c r="R41" s="31"/>
+      <c r="S41" s="31" t="s">
+        <v>189</v>
+      </c>
+      <c r="T41" s="31"/>
+      <c r="U41" s="31"/>
+      <c r="V41" s="31"/>
+      <c r="W41" s="31"/>
+      <c r="X41" s="31"/>
+      <c r="Y41" s="31"/>
+      <c r="Z41" s="31"/>
+      <c r="AA41" s="31"/>
+      <c r="AB41" s="31"/>
+      <c r="AC41" s="31"/>
+      <c r="AD41" s="31"/>
+      <c r="AE41" s="31"/>
+      <c r="AF41" s="33" t="n">
         <v>0</v>
       </c>
-      <c r="AG41" s="27"/>
-      <c r="AH41" s="27"/>
-      <c r="AI41" s="27"/>
-      <c r="AJ41" s="27"/>
-      <c r="AK41" s="27"/>
+      <c r="AG41" s="31"/>
+      <c r="AH41" s="31"/>
+      <c r="AI41" s="31"/>
+      <c r="AJ41" s="31"/>
+      <c r="AK41" s="31"/>
       <c r="AL41" s="7"/>
-      <c r="AM41" s="27"/>
+      <c r="AM41" s="31"/>
       <c r="AN41" s="7" t="n">
         <v>40</v>
       </c>
-      <c r="AO41" s="28" t="s">
-        <v>186</v>
-      </c>
-      <c r="AP41" s="27"/>
-      <c r="AQ41" s="27"/>
+      <c r="AO41" s="32" t="s">
+        <v>190</v>
+      </c>
+      <c r="AP41" s="31"/>
+      <c r="AQ41" s="31"/>
     </row>
     <row r="42" customFormat="false" ht="32.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="7" t="n">
@@ -4631,70 +4666,70 @@
       <c r="C42" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D42" s="24" t="s">
-        <v>180</v>
-      </c>
-      <c r="E42" s="26" t="s">
-        <v>165</v>
-      </c>
-      <c r="F42" s="26" t="s">
-        <v>187</v>
-      </c>
-      <c r="G42" s="26" t="s">
-        <v>188</v>
-      </c>
-      <c r="H42" s="27" t="s">
-        <v>166</v>
-      </c>
-      <c r="I42" s="28" t="s">
+      <c r="D42" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="E42" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="F42" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="G42" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="H42" s="31" t="s">
+        <v>170</v>
+      </c>
+      <c r="I42" s="32" t="s">
+        <v>193</v>
+      </c>
+      <c r="J42" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="K42" s="31"/>
+      <c r="L42" s="31"/>
+      <c r="M42" s="32"/>
+      <c r="N42" s="32"/>
+      <c r="O42" s="32" t="s">
+        <v>195</v>
+      </c>
+      <c r="P42" s="31"/>
+      <c r="Q42" s="31"/>
+      <c r="R42" s="31"/>
+      <c r="S42" s="31" t="s">
         <v>189</v>
       </c>
-      <c r="J42" s="28" t="s">
-        <v>190</v>
-      </c>
-      <c r="K42" s="27"/>
-      <c r="L42" s="27"/>
-      <c r="M42" s="28"/>
-      <c r="N42" s="28"/>
-      <c r="O42" s="28" t="s">
-        <v>191</v>
-      </c>
-      <c r="P42" s="27"/>
-      <c r="Q42" s="27"/>
-      <c r="R42" s="27"/>
-      <c r="S42" s="27" t="s">
-        <v>185</v>
-      </c>
-      <c r="T42" s="27"/>
-      <c r="U42" s="27"/>
-      <c r="V42" s="27"/>
-      <c r="W42" s="27"/>
-      <c r="X42" s="27"/>
-      <c r="Y42" s="27"/>
-      <c r="Z42" s="27"/>
-      <c r="AA42" s="27"/>
-      <c r="AB42" s="27"/>
-      <c r="AC42" s="27"/>
-      <c r="AD42" s="27"/>
-      <c r="AE42" s="27"/>
-      <c r="AF42" s="29" t="n">
+      <c r="T42" s="31"/>
+      <c r="U42" s="31"/>
+      <c r="V42" s="31"/>
+      <c r="W42" s="31"/>
+      <c r="X42" s="31"/>
+      <c r="Y42" s="31"/>
+      <c r="Z42" s="31"/>
+      <c r="AA42" s="31"/>
+      <c r="AB42" s="31"/>
+      <c r="AC42" s="31"/>
+      <c r="AD42" s="31"/>
+      <c r="AE42" s="31"/>
+      <c r="AF42" s="33" t="n">
         <v>0</v>
       </c>
-      <c r="AG42" s="27"/>
-      <c r="AH42" s="27"/>
-      <c r="AI42" s="27"/>
-      <c r="AJ42" s="27"/>
-      <c r="AK42" s="27"/>
+      <c r="AG42" s="31"/>
+      <c r="AH42" s="31"/>
+      <c r="AI42" s="31"/>
+      <c r="AJ42" s="31"/>
+      <c r="AK42" s="31"/>
       <c r="AL42" s="7"/>
-      <c r="AM42" s="27"/>
+      <c r="AM42" s="31"/>
       <c r="AN42" s="7" t="n">
         <v>41</v>
       </c>
-      <c r="AO42" s="28" t="n">
+      <c r="AO42" s="32" t="n">
         <v>37</v>
       </c>
-      <c r="AP42" s="27"/>
-      <c r="AQ42" s="27"/>
+      <c r="AP42" s="31"/>
+      <c r="AQ42" s="31"/>
     </row>
     <row r="43" customFormat="false" ht="32.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="7" t="n">
@@ -4706,70 +4741,70 @@
       <c r="C43" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D43" s="24" t="s">
-        <v>180</v>
-      </c>
-      <c r="E43" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="F43" s="26" t="s">
-        <v>192</v>
-      </c>
-      <c r="G43" s="26" t="s">
+      <c r="D43" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="E43" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="F43" s="30" t="s">
+        <v>196</v>
+      </c>
+      <c r="G43" s="30" t="s">
+        <v>197</v>
+      </c>
+      <c r="H43" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="I43" s="32" t="s">
         <v>193</v>
       </c>
-      <c r="H43" s="27" t="s">
-        <v>116</v>
-      </c>
-      <c r="I43" s="28" t="s">
+      <c r="J43" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="K43" s="31"/>
+      <c r="L43" s="31"/>
+      <c r="M43" s="32"/>
+      <c r="N43" s="32"/>
+      <c r="O43" s="32" t="s">
+        <v>198</v>
+      </c>
+      <c r="P43" s="31"/>
+      <c r="Q43" s="31"/>
+      <c r="R43" s="31"/>
+      <c r="S43" s="31" t="s">
         <v>189</v>
       </c>
-      <c r="J43" s="28" t="s">
-        <v>190</v>
-      </c>
-      <c r="K43" s="27"/>
-      <c r="L43" s="27"/>
-      <c r="M43" s="28"/>
-      <c r="N43" s="28"/>
-      <c r="O43" s="28" t="s">
-        <v>194</v>
-      </c>
-      <c r="P43" s="27"/>
-      <c r="Q43" s="27"/>
-      <c r="R43" s="27"/>
-      <c r="S43" s="27" t="s">
-        <v>185</v>
-      </c>
-      <c r="T43" s="27"/>
-      <c r="U43" s="27"/>
-      <c r="V43" s="27"/>
-      <c r="W43" s="27"/>
-      <c r="X43" s="27"/>
-      <c r="Y43" s="27"/>
-      <c r="Z43" s="27"/>
-      <c r="AA43" s="27"/>
-      <c r="AB43" s="27"/>
-      <c r="AC43" s="27"/>
-      <c r="AD43" s="27"/>
-      <c r="AE43" s="27"/>
-      <c r="AF43" s="29" t="n">
+      <c r="T43" s="31"/>
+      <c r="U43" s="31"/>
+      <c r="V43" s="31"/>
+      <c r="W43" s="31"/>
+      <c r="X43" s="31"/>
+      <c r="Y43" s="31"/>
+      <c r="Z43" s="31"/>
+      <c r="AA43" s="31"/>
+      <c r="AB43" s="31"/>
+      <c r="AC43" s="31"/>
+      <c r="AD43" s="31"/>
+      <c r="AE43" s="31"/>
+      <c r="AF43" s="33" t="n">
         <v>0</v>
       </c>
-      <c r="AG43" s="27"/>
-      <c r="AH43" s="27"/>
-      <c r="AI43" s="27"/>
-      <c r="AJ43" s="27"/>
-      <c r="AK43" s="27"/>
+      <c r="AG43" s="31"/>
+      <c r="AH43" s="31"/>
+      <c r="AI43" s="31"/>
+      <c r="AJ43" s="31"/>
+      <c r="AK43" s="31"/>
       <c r="AL43" s="7"/>
-      <c r="AM43" s="27"/>
+      <c r="AM43" s="31"/>
       <c r="AN43" s="7" t="n">
         <v>42</v>
       </c>
-      <c r="AO43" s="28" t="n">
+      <c r="AO43" s="32" t="n">
         <v>28</v>
       </c>
-      <c r="AP43" s="27"/>
-      <c r="AQ43" s="27"/>
+      <c r="AP43" s="31"/>
+      <c r="AQ43" s="31"/>
     </row>
     <row r="44" customFormat="false" ht="32.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="7" t="n">
@@ -4781,70 +4816,70 @@
       <c r="C44" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D44" s="24" t="s">
-        <v>180</v>
-      </c>
-      <c r="E44" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="F44" s="26" t="s">
-        <v>192</v>
-      </c>
-      <c r="G44" s="26" t="s">
+      <c r="D44" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="E44" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="F44" s="30" t="s">
+        <v>196</v>
+      </c>
+      <c r="G44" s="30" t="s">
+        <v>197</v>
+      </c>
+      <c r="H44" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="I44" s="32" t="s">
         <v>193</v>
       </c>
-      <c r="H44" s="27" t="s">
-        <v>121</v>
-      </c>
-      <c r="I44" s="28" t="s">
+      <c r="J44" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="K44" s="31"/>
+      <c r="L44" s="31"/>
+      <c r="M44" s="32"/>
+      <c r="N44" s="32"/>
+      <c r="O44" s="32" t="s">
+        <v>199</v>
+      </c>
+      <c r="P44" s="31"/>
+      <c r="Q44" s="31"/>
+      <c r="R44" s="31"/>
+      <c r="S44" s="31" t="s">
         <v>189</v>
       </c>
-      <c r="J44" s="28" t="s">
-        <v>190</v>
-      </c>
-      <c r="K44" s="27"/>
-      <c r="L44" s="27"/>
-      <c r="M44" s="28"/>
-      <c r="N44" s="28"/>
-      <c r="O44" s="28" t="s">
-        <v>195</v>
-      </c>
-      <c r="P44" s="27"/>
-      <c r="Q44" s="27"/>
-      <c r="R44" s="27"/>
-      <c r="S44" s="27" t="s">
-        <v>185</v>
-      </c>
-      <c r="T44" s="27"/>
-      <c r="U44" s="27"/>
-      <c r="V44" s="27"/>
-      <c r="W44" s="27"/>
-      <c r="X44" s="27"/>
-      <c r="Y44" s="27"/>
-      <c r="Z44" s="27"/>
-      <c r="AA44" s="27"/>
-      <c r="AB44" s="27"/>
-      <c r="AC44" s="27"/>
-      <c r="AD44" s="27"/>
-      <c r="AE44" s="27"/>
-      <c r="AF44" s="29" t="n">
+      <c r="T44" s="31"/>
+      <c r="U44" s="31"/>
+      <c r="V44" s="31"/>
+      <c r="W44" s="31"/>
+      <c r="X44" s="31"/>
+      <c r="Y44" s="31"/>
+      <c r="Z44" s="31"/>
+      <c r="AA44" s="31"/>
+      <c r="AB44" s="31"/>
+      <c r="AC44" s="31"/>
+      <c r="AD44" s="31"/>
+      <c r="AE44" s="31"/>
+      <c r="AF44" s="33" t="n">
         <v>0</v>
       </c>
-      <c r="AG44" s="27"/>
-      <c r="AH44" s="27"/>
-      <c r="AI44" s="27"/>
-      <c r="AJ44" s="27"/>
-      <c r="AK44" s="27"/>
+      <c r="AG44" s="31"/>
+      <c r="AH44" s="31"/>
+      <c r="AI44" s="31"/>
+      <c r="AJ44" s="31"/>
+      <c r="AK44" s="31"/>
       <c r="AL44" s="7"/>
-      <c r="AM44" s="27"/>
+      <c r="AM44" s="31"/>
       <c r="AN44" s="7" t="n">
         <v>43</v>
       </c>
-      <c r="AO44" s="28" t="n">
+      <c r="AO44" s="32" t="n">
         <v>29</v>
       </c>
-      <c r="AP44" s="27"/>
-      <c r="AQ44" s="27"/>
+      <c r="AP44" s="31"/>
+      <c r="AQ44" s="31"/>
     </row>
     <row r="45" customFormat="false" ht="32.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="7" t="n">
@@ -4856,70 +4891,70 @@
       <c r="C45" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D45" s="24" t="s">
-        <v>180</v>
-      </c>
-      <c r="E45" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="F45" s="26" t="s">
-        <v>192</v>
-      </c>
-      <c r="G45" s="26" t="s">
+      <c r="D45" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="E45" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="F45" s="30" t="s">
+        <v>196</v>
+      </c>
+      <c r="G45" s="30" t="s">
+        <v>197</v>
+      </c>
+      <c r="H45" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="I45" s="32" t="s">
         <v>193</v>
       </c>
-      <c r="H45" s="27" t="s">
-        <v>129</v>
-      </c>
-      <c r="I45" s="28" t="s">
+      <c r="J45" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="K45" s="31"/>
+      <c r="L45" s="31"/>
+      <c r="M45" s="32"/>
+      <c r="N45" s="32"/>
+      <c r="O45" s="32" t="s">
+        <v>200</v>
+      </c>
+      <c r="P45" s="31"/>
+      <c r="Q45" s="31"/>
+      <c r="R45" s="31"/>
+      <c r="S45" s="31" t="s">
         <v>189</v>
       </c>
-      <c r="J45" s="28" t="s">
-        <v>190</v>
-      </c>
-      <c r="K45" s="27"/>
-      <c r="L45" s="27"/>
-      <c r="M45" s="28"/>
-      <c r="N45" s="28"/>
-      <c r="O45" s="28" t="s">
-        <v>196</v>
-      </c>
-      <c r="P45" s="27"/>
-      <c r="Q45" s="27"/>
-      <c r="R45" s="27"/>
-      <c r="S45" s="27" t="s">
-        <v>185</v>
-      </c>
-      <c r="T45" s="27"/>
-      <c r="U45" s="27"/>
-      <c r="V45" s="27"/>
-      <c r="W45" s="27"/>
-      <c r="X45" s="27"/>
-      <c r="Y45" s="27"/>
-      <c r="Z45" s="27"/>
-      <c r="AA45" s="27"/>
-      <c r="AB45" s="27"/>
-      <c r="AC45" s="27"/>
-      <c r="AD45" s="27"/>
-      <c r="AE45" s="27"/>
-      <c r="AF45" s="29" t="n">
+      <c r="T45" s="31"/>
+      <c r="U45" s="31"/>
+      <c r="V45" s="31"/>
+      <c r="W45" s="31"/>
+      <c r="X45" s="31"/>
+      <c r="Y45" s="31"/>
+      <c r="Z45" s="31"/>
+      <c r="AA45" s="31"/>
+      <c r="AB45" s="31"/>
+      <c r="AC45" s="31"/>
+      <c r="AD45" s="31"/>
+      <c r="AE45" s="31"/>
+      <c r="AF45" s="33" t="n">
         <v>0</v>
       </c>
-      <c r="AG45" s="27"/>
-      <c r="AH45" s="27"/>
-      <c r="AI45" s="27"/>
-      <c r="AJ45" s="27"/>
-      <c r="AK45" s="27"/>
+      <c r="AG45" s="31"/>
+      <c r="AH45" s="31"/>
+      <c r="AI45" s="31"/>
+      <c r="AJ45" s="31"/>
+      <c r="AK45" s="31"/>
       <c r="AL45" s="7"/>
-      <c r="AM45" s="27"/>
+      <c r="AM45" s="31"/>
       <c r="AN45" s="7" t="n">
         <v>44</v>
       </c>
-      <c r="AO45" s="28" t="n">
+      <c r="AO45" s="32" t="n">
         <v>30</v>
       </c>
-      <c r="AP45" s="27"/>
-      <c r="AQ45" s="27"/>
+      <c r="AP45" s="31"/>
+      <c r="AQ45" s="31"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AQ41"/>
@@ -4947,17 +4982,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.81376518218623"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="180" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="30" t="s">
-        <v>161</v>
+      <c r="A1" s="34" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="180" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="30" t="s">
-        <v>156</v>
+      <c r="A2" s="34" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -4984,53 +5019,53 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.81376518218623"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="32" t="s">
-        <v>197</v>
-      </c>
-      <c r="H1" s="32" t="s">
-        <v>198</v>
-      </c>
-      <c r="I1" s="32" t="s">
+      <c r="G1" s="36" t="s">
+        <v>201</v>
+      </c>
+      <c r="H1" s="36" t="s">
+        <v>202</v>
+      </c>
+      <c r="I1" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="J1" s="32" t="s">
+      <c r="J1" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="K1" s="32" t="s">
-        <v>199</v>
-      </c>
-      <c r="L1" s="32" t="s">
+      <c r="K1" s="36" t="s">
+        <v>203</v>
+      </c>
+      <c r="L1" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="M1" s="32" t="s">
+      <c r="M1" s="36" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="33" t="s">
-        <v>200</v>
+      <c r="B4" s="37" t="s">
+        <v>204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CCRU - POS Template fix
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/Canteen PoS 2018.xlsx
+++ b/Projects/CCRU/Data/Canteen PoS 2018.xlsx
@@ -29,6 +29,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Canteen!$A$1:$AQ$41</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Canteen!$A$1:$AQ$41</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Canteen!$A$1:$AQ$41</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Canteen!$A$1:$AQ$41</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -255,16 +256,16 @@
     <t xml:space="preserve">Фанта Апельсин - 0.5л</t>
   </si>
   <si>
-    <t xml:space="preserve">Sprite - 0.33L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Спрайт - 0.33л</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fanta Orange - 0.33L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Фанта Апельсин - 0.33л</t>
+    <t xml:space="preserve">Sprite - 0.25L Slim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Спрайт - 0.25л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fanta Orange - 0.25L Slim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Фанта Апельсин – 0.25л</t>
   </si>
   <si>
     <t xml:space="preserve">STANDARD 2</t>
@@ -938,9 +939,9 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
@@ -950,9 +951,9 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+      <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
@@ -1094,17 +1095,17 @@
   </sheetPr>
   <dimension ref="A1:AR45"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="L25" activeCellId="0" sqref="L25"/>
+      <selection pane="bottomLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="32.45"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="1" width="15.5465587044534"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="43.4615384615385"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="15.5465587044534"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="1" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="45.417004048583"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="16.2834008097166"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="62.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1770,7 +1771,7 @@
         <v>47</v>
       </c>
       <c r="F8" s="8"/>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="20" t="s">
         <v>69</v>
       </c>
       <c r="H8" s="13" t="s">
@@ -1785,11 +1786,11 @@
       </c>
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
-      <c r="N8" s="8" t="s">
+      <c r="N8" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="O8" s="9" t="n">
-        <v>5449000014535</v>
+      <c r="O8" s="22" t="n">
+        <v>5449000000729</v>
       </c>
       <c r="P8" s="8"/>
       <c r="Q8" s="8"/>
@@ -1858,7 +1859,7 @@
         <v>47</v>
       </c>
       <c r="F9" s="8"/>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="20" t="s">
         <v>71</v>
       </c>
       <c r="H9" s="13" t="s">
@@ -1873,11 +1874,11 @@
       </c>
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
-      <c r="N9" s="8" t="s">
+      <c r="N9" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="O9" s="9" t="n">
-        <v>5449000011527</v>
+      <c r="O9" s="22" t="n">
+        <v>5449000000712</v>
       </c>
       <c r="P9" s="8"/>
       <c r="Q9" s="8"/>
@@ -3306,10 +3307,10 @@
         <v>73</v>
       </c>
       <c r="F26" s="8"/>
-      <c r="G26" s="20" t="s">
+      <c r="G26" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="H26" s="20" t="s">
+      <c r="H26" s="23" t="s">
         <v>110</v>
       </c>
       <c r="I26" s="8" t="s">
@@ -3394,10 +3395,10 @@
         <v>73</v>
       </c>
       <c r="F27" s="8"/>
-      <c r="G27" s="23" t="s">
+      <c r="G27" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="H27" s="20" t="s">
+      <c r="H27" s="23" t="s">
         <v>114</v>
       </c>
       <c r="I27" s="8" t="s">
@@ -4976,13 +4977,13 @@
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.81376518218623"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.1417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="180" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5013,13 +5014,13 @@
   </sheetPr>
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.81376518218623"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.1417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
PROS-7431 - CCRU - KPI templates update
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/Canteen PoS 2018.xlsx
+++ b/Projects/CCRU/Data/Canteen PoS 2018.xlsx
@@ -13,7 +13,7 @@
     <sheet name="Alcomarket" sheetId="3" state="hidden" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Canteen!$A$1:$AQ$45</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Canteen!$A$1:$AQ$41</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0" vbProcedure="false">Canteen!$A$1:$AQ$41</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0" vbProcedure="false">Canteen!$A$1:$AQ$41</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0" vbProcedure="false">Canteen!$A$1:$AQ$41</definedName>
@@ -25,13 +25,14 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Canteen!$A$1:$AQ$41</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Canteen!$A$1:$AQ$41</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Canteen!$A$1:$AQ$41</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Canteen!$A$1:$AQ$41</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Canteen!$A$1:$AQ$45</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Canteen!$A$1:$AQ$41</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Canteen!$A$1:$AQ$41</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Canteen!$A$1:$AQ$41</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Canteen!$A$1:$AQ$41</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Canteen!$A$1:$AQ$41</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Canteen!$A$1:$AQ$41</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Canteen!$A$1:$AQ$41</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="225">
   <si>
     <t xml:space="preserve">Sorting</t>
   </si>
@@ -329,16 +330,25 @@
     <t xml:space="preserve">Фьюз Лимон - 0.33л</t>
   </si>
   <si>
+    <t xml:space="preserve">5449000045720, 5449000236777</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fuze Berry - 0.5L</t>
   </si>
   <si>
     <t xml:space="preserve">Фьюз Лесн.ягоды - 0.5л</t>
   </si>
   <si>
+    <t xml:space="preserve">5449000193124, 5449000259455</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fuze Lemon - 0.5L</t>
   </si>
   <si>
     <t xml:space="preserve">Фьюз Лимон - 0.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5449000189301, 5449000235947</t>
   </si>
   <si>
     <t xml:space="preserve">Fuze Green Strawberry-Raspberry - 0.5L</t>
@@ -742,11 +752,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
     <numFmt numFmtId="166" formatCode="0%"/>
     <numFmt numFmtId="167" formatCode="0.0%"/>
+    <numFmt numFmtId="168" formatCode="@"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -754,6 +765,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -774,17 +786,20 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -792,6 +807,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -799,9 +815,10 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -816,12 +833,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FFFF9900"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor rgb="FFC0C0C0"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -841,6 +864,13 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -900,10 +930,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -931,6 +957,10 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -943,7 +973,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1014,7 +1044,7 @@
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF92D050"/>
-      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFFC000"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
@@ -1046,34 +1076,34 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="AA13" activeCellId="0" sqref="AA13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="27.95"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.0607287449393"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.6842105263158"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.5627530364372"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.6558704453441"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.0971659919028"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="7.93522267206478"/>
-    <col collapsed="false" hidden="false" max="10" min="7" style="0" width="16.753036437247"/>
-    <col collapsed="false" hidden="false" max="13" min="11" style="1" width="7.93522267206478"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="1" width="50.1255060728745"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="13.2955465587045"/>
-    <col collapsed="false" hidden="false" max="18" min="17" style="1" width="17.0445344129555"/>
-    <col collapsed="false" hidden="false" max="20" min="19" style="1" width="12.1983805668016"/>
-    <col collapsed="false" hidden="false" max="23" min="21" style="1" width="11.753036437247"/>
-    <col collapsed="false" hidden="false" max="26" min="24" style="1" width="11.6113360323887"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="18.2226720647773"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="17.0445344129555"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="22.6396761133603"/>
-    <col collapsed="false" hidden="false" max="31" min="30" style="1" width="11.6113360323887"/>
-    <col collapsed="false" hidden="false" max="34" min="32" style="1" width="17.7813765182186"/>
-    <col collapsed="false" hidden="false" max="42" min="35" style="1" width="23.2226720647773"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="1" width="40.2753036437247"/>
-    <col collapsed="false" hidden="false" max="1009" min="44" style="1" width="9.1417004048583"/>
-    <col collapsed="false" hidden="false" max="1025" min="1010" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.6761133603239"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.7125506072875"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.1417004048583"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="7.92712550607287"/>
+    <col collapsed="false" hidden="false" max="10" min="7" style="0" width="16.9230769230769"/>
+    <col collapsed="false" hidden="false" max="13" min="11" style="1" width="7.92712550607287"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="1" width="50.5587044534413"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="18" min="17" style="1" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="20" min="19" style="1" width="12.3198380566802"/>
+    <col collapsed="false" hidden="false" max="23" min="21" style="1" width="11.7813765182186"/>
+    <col collapsed="false" hidden="false" max="26" min="24" style="1" width="11.5708502024291"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="31" min="30" style="1" width="11.5708502024291"/>
+    <col collapsed="false" hidden="false" max="34" min="32" style="1" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="42" min="35" style="1" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="1" width="40.5991902834008"/>
+    <col collapsed="false" hidden="false" max="1009" min="44" style="1" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1025" min="1010" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="45.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1241,22 +1271,22 @@
       <c r="F2" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="5" t="s">
         <v>50</v>
       </c>
       <c r="K2" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="6" t="s">
         <v>51</v>
       </c>
       <c r="M2" s="5"/>
@@ -1282,13 +1312,13 @@
       <c r="Y2" s="5"/>
       <c r="Z2" s="5"/>
       <c r="AA2" s="5"/>
-      <c r="AB2" s="8"/>
+      <c r="AB2" s="7"/>
       <c r="AC2" s="5"/>
       <c r="AD2" s="5"/>
       <c r="AE2" s="5"/>
-      <c r="AF2" s="8"/>
-      <c r="AG2" s="8"/>
-      <c r="AH2" s="8"/>
+      <c r="AF2" s="7"/>
+      <c r="AG2" s="7"/>
+      <c r="AH2" s="7"/>
       <c r="AI2" s="5"/>
       <c r="AJ2" s="5"/>
       <c r="AK2" s="5"/>
@@ -1318,16 +1348,16 @@
       <c r="F3" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="5" t="s">
         <v>50</v>
       </c>
       <c r="K3" s="5" t="n">
@@ -1340,10 +1370,10 @@
       <c r="N3" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="O3" s="9" t="s">
+      <c r="O3" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="P3" s="10" t="n">
+      <c r="P3" s="9" t="n">
         <v>0.024996</v>
       </c>
       <c r="Q3" s="5" t="s">
@@ -1367,7 +1397,7 @@
       <c r="Y3" s="5"/>
       <c r="Z3" s="5"/>
       <c r="AA3" s="5"/>
-      <c r="AB3" s="8" t="n">
+      <c r="AB3" s="7" t="n">
         <v>5449000008046</v>
       </c>
       <c r="AC3" s="5" t="s">
@@ -1375,9 +1405,9 @@
       </c>
       <c r="AD3" s="5"/>
       <c r="AE3" s="5"/>
-      <c r="AF3" s="8"/>
-      <c r="AG3" s="8"/>
-      <c r="AH3" s="8"/>
+      <c r="AF3" s="7"/>
+      <c r="AG3" s="7"/>
+      <c r="AH3" s="7"/>
       <c r="AI3" s="5"/>
       <c r="AJ3" s="5" t="s">
         <v>60</v>
@@ -1411,16 +1441,16 @@
       <c r="F4" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="J4" s="5" t="s">
         <v>50</v>
       </c>
       <c r="K4" s="5" t="n">
@@ -1433,10 +1463,10 @@
       <c r="N4" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="O4" s="9" t="s">
+      <c r="O4" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="P4" s="10" t="n">
+      <c r="P4" s="9" t="n">
         <v>0.024996</v>
       </c>
       <c r="Q4" s="5" t="s">
@@ -1460,7 +1490,7 @@
       <c r="Y4" s="5"/>
       <c r="Z4" s="5"/>
       <c r="AA4" s="5"/>
-      <c r="AB4" s="8" t="n">
+      <c r="AB4" s="7" t="n">
         <v>5449000020987</v>
       </c>
       <c r="AC4" s="5" t="s">
@@ -1468,9 +1498,9 @@
       </c>
       <c r="AD4" s="5"/>
       <c r="AE4" s="5"/>
-      <c r="AF4" s="8"/>
-      <c r="AG4" s="8"/>
-      <c r="AH4" s="8"/>
+      <c r="AF4" s="7"/>
+      <c r="AG4" s="7"/>
+      <c r="AH4" s="7"/>
       <c r="AI4" s="5"/>
       <c r="AJ4" s="5" t="s">
         <v>60</v>
@@ -1504,32 +1534,32 @@
       <c r="F5" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="5" t="s">
         <v>50</v>
       </c>
       <c r="K5" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="L5" s="11"/>
+      <c r="L5" s="10"/>
       <c r="M5" s="5" t="n">
         <v>1</v>
       </c>
       <c r="N5" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="O5" s="9" t="s">
+      <c r="O5" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="P5" s="12" t="n">
+      <c r="P5" s="11" t="n">
         <v>0.014004</v>
       </c>
       <c r="Q5" s="5" t="s">
@@ -1545,15 +1575,15 @@
       <c r="U5" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="V5" s="11"/>
-      <c r="W5" s="11"/>
+      <c r="V5" s="10"/>
+      <c r="W5" s="10"/>
       <c r="X5" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="Y5" s="11"/>
-      <c r="Z5" s="11"/>
-      <c r="AA5" s="11"/>
-      <c r="AB5" s="8" t="n">
+      <c r="Y5" s="10"/>
+      <c r="Z5" s="10"/>
+      <c r="AA5" s="10"/>
+      <c r="AB5" s="7" t="n">
         <v>54491472</v>
       </c>
       <c r="AC5" s="5" t="s">
@@ -1561,9 +1591,9 @@
       </c>
       <c r="AD5" s="5"/>
       <c r="AE5" s="5"/>
-      <c r="AF5" s="13"/>
-      <c r="AG5" s="13"/>
-      <c r="AH5" s="13"/>
+      <c r="AF5" s="12"/>
+      <c r="AG5" s="12"/>
+      <c r="AH5" s="12"/>
       <c r="AI5" s="5"/>
       <c r="AJ5" s="5" t="s">
         <v>60</v>
@@ -1576,7 +1606,7 @@
       <c r="AN5" s="5"/>
       <c r="AO5" s="5"/>
       <c r="AP5" s="5"/>
-      <c r="AQ5" s="11"/>
+      <c r="AQ5" s="10"/>
     </row>
     <row r="6" customFormat="false" ht="27.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="n">
@@ -1597,16 +1627,16 @@
       <c r="F6" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="J6" s="5" t="s">
         <v>50</v>
       </c>
       <c r="K6" s="5" t="n">
@@ -1619,10 +1649,10 @@
       <c r="N6" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="O6" s="9" t="s">
+      <c r="O6" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="P6" s="10" t="n">
+      <c r="P6" s="9" t="n">
         <v>0.014004</v>
       </c>
       <c r="Q6" s="5" t="s">
@@ -1646,7 +1676,7 @@
       <c r="Y6" s="5"/>
       <c r="Z6" s="5"/>
       <c r="AA6" s="5"/>
-      <c r="AB6" s="8" t="n">
+      <c r="AB6" s="7" t="n">
         <v>54491069</v>
       </c>
       <c r="AC6" s="5" t="s">
@@ -1654,9 +1684,9 @@
       </c>
       <c r="AD6" s="5"/>
       <c r="AE6" s="5"/>
-      <c r="AF6" s="8"/>
-      <c r="AG6" s="8"/>
-      <c r="AH6" s="8"/>
+      <c r="AF6" s="7"/>
+      <c r="AG6" s="7"/>
+      <c r="AH6" s="7"/>
       <c r="AI6" s="5"/>
       <c r="AJ6" s="5" t="s">
         <v>60</v>
@@ -1690,16 +1720,16 @@
       <c r="F7" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="I7" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="J7" s="5" t="s">
         <v>50</v>
       </c>
       <c r="K7" s="5" t="n">
@@ -1712,10 +1742,10 @@
       <c r="N7" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="O7" s="9" t="s">
+      <c r="O7" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="P7" s="10" t="n">
+      <c r="P7" s="9" t="n">
         <v>0.014004</v>
       </c>
       <c r="Q7" s="5" t="s">
@@ -1739,7 +1769,7 @@
       <c r="Y7" s="5"/>
       <c r="Z7" s="5"/>
       <c r="AA7" s="5"/>
-      <c r="AB7" s="8" t="n">
+      <c r="AB7" s="7" t="n">
         <v>40822938</v>
       </c>
       <c r="AC7" s="5" t="s">
@@ -1747,9 +1777,9 @@
       </c>
       <c r="AD7" s="5"/>
       <c r="AE7" s="5"/>
-      <c r="AF7" s="8"/>
-      <c r="AG7" s="8"/>
-      <c r="AH7" s="8"/>
+      <c r="AF7" s="7"/>
+      <c r="AG7" s="7"/>
+      <c r="AH7" s="7"/>
       <c r="AI7" s="5"/>
       <c r="AJ7" s="5" t="s">
         <v>60</v>
@@ -1783,16 +1813,16 @@
       <c r="F8" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="I8" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="J8" s="5" t="s">
         <v>50</v>
       </c>
       <c r="K8" s="5" t="n">
@@ -1805,10 +1835,10 @@
       <c r="N8" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="O8" s="9" t="s">
+      <c r="O8" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="P8" s="10" t="n">
+      <c r="P8" s="9" t="n">
         <v>0.014004</v>
       </c>
       <c r="Q8" s="5" t="s">
@@ -1832,7 +1862,7 @@
       <c r="Y8" s="5"/>
       <c r="Z8" s="5"/>
       <c r="AA8" s="5"/>
-      <c r="AB8" s="8" t="n">
+      <c r="AB8" s="7" t="n">
         <v>5449000000729</v>
       </c>
       <c r="AC8" s="5" t="s">
@@ -1876,16 +1906,16 @@
       <c r="F9" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="I9" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="J9" s="5" t="s">
         <v>50</v>
       </c>
       <c r="K9" s="5" t="n">
@@ -1898,10 +1928,10 @@
       <c r="N9" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="O9" s="9" t="s">
+      <c r="O9" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="P9" s="10" t="n">
+      <c r="P9" s="9" t="n">
         <v>0.013992</v>
       </c>
       <c r="Q9" s="5" t="s">
@@ -1925,7 +1955,7 @@
       <c r="Y9" s="5"/>
       <c r="Z9" s="5"/>
       <c r="AA9" s="5"/>
-      <c r="AB9" s="8" t="n">
+      <c r="AB9" s="7" t="n">
         <v>5449000000712</v>
       </c>
       <c r="AC9" s="5" t="s">
@@ -1969,22 +1999,22 @@
       <c r="F10" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="I10" s="6" t="s">
+      <c r="I10" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="J10" s="6" t="s">
+      <c r="J10" s="5" t="s">
         <v>76</v>
       </c>
       <c r="K10" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="L10" s="7" t="s">
+      <c r="L10" s="6" t="s">
         <v>77</v>
       </c>
       <c r="M10" s="5"/>
@@ -2010,13 +2040,13 @@
       <c r="Y10" s="5"/>
       <c r="Z10" s="5"/>
       <c r="AA10" s="5"/>
-      <c r="AB10" s="8"/>
+      <c r="AB10" s="7"/>
       <c r="AC10" s="5"/>
       <c r="AD10" s="5"/>
       <c r="AE10" s="5"/>
-      <c r="AF10" s="8"/>
-      <c r="AG10" s="8"/>
-      <c r="AH10" s="8"/>
+      <c r="AF10" s="7"/>
+      <c r="AG10" s="7"/>
+      <c r="AH10" s="7"/>
       <c r="AI10" s="5"/>
       <c r="AJ10" s="5"/>
       <c r="AK10" s="5"/>
@@ -2046,16 +2076,16 @@
       <c r="F11" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="I11" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="J11" s="6" t="s">
+      <c r="J11" s="5" t="s">
         <v>76</v>
       </c>
       <c r="K11" s="5" t="n">
@@ -2068,10 +2098,10 @@
       <c r="N11" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="O11" s="9" t="s">
+      <c r="O11" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="P11" s="10" t="n">
+      <c r="P11" s="9" t="n">
         <v>0.025004</v>
       </c>
       <c r="Q11" s="5" t="s">
@@ -2095,7 +2125,7 @@
       <c r="Y11" s="5"/>
       <c r="Z11" s="5"/>
       <c r="AA11" s="5"/>
-      <c r="AB11" s="8" t="n">
+      <c r="AB11" s="7" t="n">
         <v>90494956</v>
       </c>
       <c r="AC11" s="5" t="s">
@@ -2139,16 +2169,16 @@
       <c r="F12" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="I12" s="6" t="s">
+      <c r="I12" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="J12" s="6" t="s">
+      <c r="J12" s="5" t="s">
         <v>76</v>
       </c>
       <c r="K12" s="5" t="n">
@@ -2161,10 +2191,10 @@
       <c r="N12" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="O12" s="9" t="s">
+      <c r="O12" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="P12" s="10" t="n">
+      <c r="P12" s="9" t="n">
         <v>0.025004</v>
       </c>
       <c r="Q12" s="5" t="s">
@@ -2188,7 +2218,7 @@
       <c r="Y12" s="5"/>
       <c r="Z12" s="5"/>
       <c r="AA12" s="5"/>
-      <c r="AB12" s="8" t="n">
+      <c r="AB12" s="7" t="n">
         <v>40822426</v>
       </c>
       <c r="AC12" s="5" t="s">
@@ -2232,16 +2262,16 @@
       <c r="F13" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="I13" s="6" t="s">
+      <c r="I13" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="J13" s="6" t="s">
+      <c r="J13" s="5" t="s">
         <v>76</v>
       </c>
       <c r="K13" s="5" t="n">
@@ -2254,10 +2284,10 @@
       <c r="N13" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="O13" s="9" t="s">
+      <c r="O13" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="P13" s="10" t="n">
+      <c r="P13" s="9" t="n">
         <v>0.012992</v>
       </c>
       <c r="Q13" s="5" t="s">
@@ -2281,7 +2311,7 @@
       <c r="Y13" s="5"/>
       <c r="Z13" s="5"/>
       <c r="AA13" s="5"/>
-      <c r="AB13" s="8" t="n">
+      <c r="AB13" s="7" t="n">
         <v>90494406</v>
       </c>
       <c r="AC13" s="5" t="s">
@@ -2325,22 +2355,22 @@
       <c r="F14" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G14" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="H14" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="I14" s="6" t="s">
+      <c r="I14" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="J14" s="6" t="s">
+      <c r="J14" s="5" t="s">
         <v>86</v>
       </c>
       <c r="K14" s="5" t="n">
         <v>13</v>
       </c>
-      <c r="L14" s="7" t="s">
+      <c r="L14" s="6" t="s">
         <v>87</v>
       </c>
       <c r="M14" s="5"/>
@@ -2366,13 +2396,13 @@
       <c r="Y14" s="5"/>
       <c r="Z14" s="5"/>
       <c r="AA14" s="5"/>
-      <c r="AB14" s="8"/>
+      <c r="AB14" s="7"/>
       <c r="AC14" s="5"/>
       <c r="AD14" s="5"/>
       <c r="AE14" s="5"/>
-      <c r="AF14" s="8"/>
-      <c r="AG14" s="8"/>
-      <c r="AH14" s="8"/>
+      <c r="AF14" s="7"/>
+      <c r="AG14" s="7"/>
+      <c r="AH14" s="7"/>
       <c r="AI14" s="5"/>
       <c r="AJ14" s="5"/>
       <c r="AK14" s="5"/>
@@ -2402,16 +2432,16 @@
       <c r="F15" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H15" s="6" t="s">
+      <c r="H15" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="I15" s="6" t="s">
+      <c r="I15" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="J15" s="6" t="s">
+      <c r="J15" s="5" t="s">
         <v>86</v>
       </c>
       <c r="K15" s="5" t="n">
@@ -2424,10 +2454,10 @@
       <c r="N15" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="O15" s="9" t="s">
+      <c r="O15" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="P15" s="10" t="n">
+      <c r="P15" s="9" t="n">
         <v>0.025004</v>
       </c>
       <c r="Q15" s="5" t="s">
@@ -2451,8 +2481,8 @@
       <c r="Y15" s="5"/>
       <c r="Z15" s="5"/>
       <c r="AA15" s="5"/>
-      <c r="AB15" s="8" t="n">
-        <v>5449000045720</v>
+      <c r="AB15" s="13" t="s">
+        <v>91</v>
       </c>
       <c r="AC15" s="5" t="s">
         <v>89</v>
@@ -2495,16 +2525,16 @@
       <c r="F16" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="H16" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="I16" s="6" t="s">
+      <c r="I16" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="J16" s="6" t="s">
+      <c r="J16" s="5" t="s">
         <v>86</v>
       </c>
       <c r="K16" s="5" t="n">
@@ -2515,12 +2545,12 @@
         <v>13</v>
       </c>
       <c r="N16" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="O16" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="P16" s="10" t="n">
+      <c r="O16" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="P16" s="9" t="n">
         <v>0.012992</v>
       </c>
       <c r="Q16" s="5" t="s">
@@ -2544,11 +2574,11 @@
       <c r="Y16" s="5"/>
       <c r="Z16" s="5"/>
       <c r="AA16" s="5"/>
-      <c r="AB16" s="8" t="n">
-        <v>5449000193124</v>
+      <c r="AB16" s="13" t="s">
+        <v>94</v>
       </c>
       <c r="AC16" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AD16" s="5"/>
       <c r="AE16" s="5"/>
@@ -2588,16 +2618,16 @@
       <c r="F17" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G17" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H17" s="6" t="s">
+      <c r="H17" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="I17" s="6" t="s">
+      <c r="I17" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="J17" s="6" t="s">
+      <c r="J17" s="5" t="s">
         <v>86</v>
       </c>
       <c r="K17" s="5" t="n">
@@ -2608,12 +2638,12 @@
         <v>13</v>
       </c>
       <c r="N17" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="O17" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="P17" s="10" t="n">
+        <v>95</v>
+      </c>
+      <c r="O17" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="P17" s="9" t="n">
         <v>0.012992</v>
       </c>
       <c r="Q17" s="5" t="s">
@@ -2637,11 +2667,11 @@
       <c r="Y17" s="5"/>
       <c r="Z17" s="5"/>
       <c r="AA17" s="5"/>
-      <c r="AB17" s="8" t="n">
-        <v>5449000189301</v>
+      <c r="AB17" s="13" t="s">
+        <v>97</v>
       </c>
       <c r="AC17" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="AD17" s="5"/>
       <c r="AE17" s="5"/>
@@ -2681,16 +2711,16 @@
       <c r="F18" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="G18" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H18" s="6" t="s">
+      <c r="H18" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="I18" s="6" t="s">
+      <c r="I18" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="J18" s="6" t="s">
+      <c r="J18" s="5" t="s">
         <v>86</v>
       </c>
       <c r="K18" s="5" t="n">
@@ -2701,12 +2731,12 @@
         <v>13</v>
       </c>
       <c r="N18" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="O18" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="P18" s="10" t="n">
+        <v>98</v>
+      </c>
+      <c r="O18" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="P18" s="9" t="n">
         <v>0.012012</v>
       </c>
       <c r="Q18" s="5" t="s">
@@ -2730,11 +2760,11 @@
       <c r="Y18" s="5"/>
       <c r="Z18" s="5"/>
       <c r="AA18" s="5"/>
-      <c r="AB18" s="8" t="n">
+      <c r="AB18" s="7" t="n">
         <v>5449000233615</v>
       </c>
       <c r="AC18" s="5" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="AD18" s="5"/>
       <c r="AE18" s="5"/>
@@ -2774,30 +2804,30 @@
       <c r="F19" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="G19" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H19" s="6" t="s">
+      <c r="H19" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="I19" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="J19" s="6" t="s">
-        <v>98</v>
+      <c r="I19" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>101</v>
       </c>
       <c r="K19" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="L19" s="7" t="s">
-        <v>99</v>
+      <c r="L19" s="6" t="s">
+        <v>102</v>
       </c>
       <c r="M19" s="5"/>
       <c r="N19" s="5" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="O19" s="5" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="P19" s="5"/>
       <c r="Q19" s="5" t="s">
@@ -2815,13 +2845,13 @@
       <c r="Y19" s="5"/>
       <c r="Z19" s="5"/>
       <c r="AA19" s="5"/>
-      <c r="AB19" s="8"/>
+      <c r="AB19" s="7"/>
       <c r="AC19" s="5"/>
       <c r="AD19" s="5"/>
       <c r="AE19" s="5"/>
-      <c r="AF19" s="8"/>
-      <c r="AG19" s="8"/>
-      <c r="AH19" s="8"/>
+      <c r="AF19" s="7"/>
+      <c r="AG19" s="7"/>
+      <c r="AH19" s="7"/>
       <c r="AI19" s="5"/>
       <c r="AJ19" s="5"/>
       <c r="AK19" s="5"/>
@@ -2851,17 +2881,17 @@
       <c r="F20" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="G20" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="H20" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="I20" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="J20" s="6" t="s">
-        <v>98</v>
+      <c r="I20" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>101</v>
       </c>
       <c r="K20" s="5" t="n">
         <v>19</v>
@@ -2871,12 +2901,12 @@
         <v>18</v>
       </c>
       <c r="N20" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="O20" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="P20" s="10" t="n">
+        <v>104</v>
+      </c>
+      <c r="O20" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="P20" s="9" t="n">
         <v>0.025004</v>
       </c>
       <c r="Q20" s="5" t="s">
@@ -2900,11 +2930,11 @@
       <c r="Y20" s="5"/>
       <c r="Z20" s="5"/>
       <c r="AA20" s="5"/>
-      <c r="AB20" s="8" t="n">
+      <c r="AB20" s="7" t="n">
         <v>4607174579309</v>
       </c>
       <c r="AC20" s="5" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="AD20" s="5"/>
       <c r="AE20" s="5"/>
@@ -2944,17 +2974,17 @@
       <c r="F21" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G21" s="6" t="s">
+      <c r="G21" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H21" s="6" t="s">
+      <c r="H21" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="I21" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="J21" s="6" t="s">
-        <v>98</v>
+      <c r="I21" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>101</v>
       </c>
       <c r="K21" s="5" t="n">
         <v>20</v>
@@ -2964,12 +2994,12 @@
         <v>18</v>
       </c>
       <c r="N21" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="O21" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="P21" s="10" t="n">
+        <v>106</v>
+      </c>
+      <c r="O21" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="P21" s="9" t="n">
         <v>0.025004</v>
       </c>
       <c r="Q21" s="5" t="s">
@@ -2993,11 +3023,11 @@
       <c r="Y21" s="5"/>
       <c r="Z21" s="5"/>
       <c r="AA21" s="5"/>
-      <c r="AB21" s="8" t="n">
+      <c r="AB21" s="7" t="n">
         <v>4607174577787</v>
       </c>
       <c r="AC21" s="5" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="AD21" s="5"/>
       <c r="AE21" s="5"/>
@@ -3037,17 +3067,17 @@
       <c r="F22" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G22" s="6" t="s">
+      <c r="G22" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H22" s="6" t="s">
+      <c r="H22" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="I22" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="J22" s="6" t="s">
-        <v>98</v>
+      <c r="I22" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>101</v>
       </c>
       <c r="K22" s="5" t="n">
         <v>21</v>
@@ -3057,12 +3087,12 @@
         <v>18</v>
       </c>
       <c r="N22" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="O22" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="P22" s="10" t="n">
+        <v>108</v>
+      </c>
+      <c r="O22" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="P22" s="9" t="n">
         <v>0.025004</v>
       </c>
       <c r="Q22" s="5" t="s">
@@ -3086,11 +3116,11 @@
       <c r="Y22" s="5"/>
       <c r="Z22" s="5"/>
       <c r="AA22" s="5"/>
-      <c r="AB22" s="8" t="n">
+      <c r="AB22" s="7" t="n">
         <v>4607174579286</v>
       </c>
       <c r="AC22" s="5" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="AD22" s="5"/>
       <c r="AE22" s="5"/>
@@ -3130,17 +3160,17 @@
       <c r="F23" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G23" s="6" t="s">
+      <c r="G23" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H23" s="6" t="s">
+      <c r="H23" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="I23" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="J23" s="6" t="s">
-        <v>98</v>
+      <c r="I23" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>101</v>
       </c>
       <c r="K23" s="5" t="n">
         <v>22</v>
@@ -3150,12 +3180,12 @@
         <v>18</v>
       </c>
       <c r="N23" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="O23" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="P23" s="10" t="n">
+        <v>110</v>
+      </c>
+      <c r="O23" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="P23" s="9" t="n">
         <v>0.025004</v>
       </c>
       <c r="Q23" s="5" t="s">
@@ -3179,11 +3209,11 @@
       <c r="Y23" s="5"/>
       <c r="Z23" s="5"/>
       <c r="AA23" s="5"/>
-      <c r="AB23" s="8" t="n">
+      <c r="AB23" s="7" t="n">
         <v>4607174579323</v>
       </c>
       <c r="AC23" s="5" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="AD23" s="5"/>
       <c r="AE23" s="5"/>
@@ -3223,17 +3253,17 @@
       <c r="F24" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G24" s="6" t="s">
+      <c r="G24" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H24" s="6" t="s">
+      <c r="H24" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="I24" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="J24" s="6" t="s">
-        <v>98</v>
+      <c r="I24" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>101</v>
       </c>
       <c r="K24" s="5" t="n">
         <v>23</v>
@@ -3243,12 +3273,12 @@
         <v>18</v>
       </c>
       <c r="N24" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="O24" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="P24" s="10" t="n">
+        <v>112</v>
+      </c>
+      <c r="O24" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="P24" s="9" t="n">
         <v>0.012012</v>
       </c>
       <c r="Q24" s="5" t="s">
@@ -3272,11 +3302,11 @@
       <c r="Y24" s="5"/>
       <c r="Z24" s="5"/>
       <c r="AA24" s="5"/>
-      <c r="AB24" s="8" t="n">
+      <c r="AB24" s="7" t="n">
         <v>4607174579729</v>
       </c>
       <c r="AC24" s="5" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="AD24" s="5"/>
       <c r="AE24" s="5"/>
@@ -3316,17 +3346,17 @@
       <c r="F25" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G25" s="6" t="s">
+      <c r="G25" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H25" s="6" t="s">
+      <c r="H25" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="I25" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="J25" s="6" t="s">
-        <v>98</v>
+      <c r="I25" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>101</v>
       </c>
       <c r="K25" s="5" t="n">
         <v>24</v>
@@ -3335,13 +3365,13 @@
       <c r="M25" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="N25" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="O25" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="P25" s="10" t="n">
+      <c r="N25" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="O25" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="P25" s="9" t="n">
         <v>0.012012</v>
       </c>
       <c r="Q25" s="5" t="s">
@@ -3365,11 +3395,11 @@
       <c r="Y25" s="5"/>
       <c r="Z25" s="5"/>
       <c r="AA25" s="5"/>
-      <c r="AB25" s="8" t="n">
+      <c r="AB25" s="7" t="n">
         <v>4607174579248</v>
       </c>
       <c r="AC25" s="5" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="AD25" s="5"/>
       <c r="AE25" s="5"/>
@@ -3409,17 +3439,17 @@
       <c r="F26" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G26" s="6" t="s">
+      <c r="G26" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H26" s="6" t="s">
+      <c r="H26" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="I26" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="J26" s="6" t="s">
-        <v>98</v>
+      <c r="I26" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>101</v>
       </c>
       <c r="K26" s="5" t="n">
         <v>25</v>
@@ -3428,13 +3458,13 @@
       <c r="M26" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="N26" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="O26" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="P26" s="10" t="n">
+      <c r="N26" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="O26" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="P26" s="9" t="n">
         <v>0.009996</v>
       </c>
       <c r="Q26" s="5" t="s">
@@ -3458,11 +3488,11 @@
       <c r="Y26" s="5"/>
       <c r="Z26" s="5"/>
       <c r="AA26" s="5"/>
-      <c r="AB26" s="8" t="s">
-        <v>115</v>
+      <c r="AB26" s="7" t="s">
+        <v>118</v>
       </c>
       <c r="AC26" s="5" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="AD26" s="5"/>
       <c r="AE26" s="5"/>
@@ -3502,17 +3532,17 @@
       <c r="F27" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G27" s="6" t="s">
+      <c r="G27" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H27" s="6" t="s">
+      <c r="H27" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="I27" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="J27" s="6" t="s">
-        <v>98</v>
+      <c r="I27" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>101</v>
       </c>
       <c r="K27" s="5" t="n">
         <v>26</v>
@@ -3522,12 +3552,12 @@
         <v>18</v>
       </c>
       <c r="N27" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="O27" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="P27" s="10" t="n">
+        <v>120</v>
+      </c>
+      <c r="O27" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="P27" s="9" t="n">
         <v>0.009996</v>
       </c>
       <c r="Q27" s="5" t="s">
@@ -3551,11 +3581,11 @@
       <c r="Y27" s="5"/>
       <c r="Z27" s="5"/>
       <c r="AA27" s="5"/>
-      <c r="AB27" s="8" t="s">
-        <v>119</v>
+      <c r="AB27" s="7" t="s">
+        <v>122</v>
       </c>
       <c r="AC27" s="5" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="AD27" s="5"/>
       <c r="AE27" s="5"/>
@@ -3595,17 +3625,17 @@
       <c r="F28" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G28" s="6" t="s">
+      <c r="G28" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H28" s="6" t="s">
+      <c r="H28" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="I28" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="J28" s="6" t="s">
-        <v>98</v>
+      <c r="I28" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>101</v>
       </c>
       <c r="K28" s="5" t="n">
         <v>27</v>
@@ -3615,12 +3645,12 @@
         <v>18</v>
       </c>
       <c r="N28" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="O28" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="P28" s="10" t="n">
+        <v>124</v>
+      </c>
+      <c r="O28" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="P28" s="9" t="n">
         <v>0.009968</v>
       </c>
       <c r="Q28" s="5" t="s">
@@ -3644,11 +3674,11 @@
       <c r="Y28" s="5"/>
       <c r="Z28" s="5"/>
       <c r="AA28" s="5"/>
-      <c r="AB28" s="8" t="n">
+      <c r="AB28" s="7" t="n">
         <v>4607174579262</v>
       </c>
       <c r="AC28" s="5" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="AD28" s="5"/>
       <c r="AE28" s="5"/>
@@ -3677,7 +3707,7 @@
         <v>43</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>45</v>
@@ -3688,17 +3718,17 @@
       <c r="F29" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="G29" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="H29" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="I29" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="J29" s="6" t="s">
+      <c r="G29" s="5" t="s">
         <v>127</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>130</v>
       </c>
       <c r="K29" s="5" t="n">
         <v>28</v>
@@ -3706,23 +3736,23 @@
       <c r="L29" s="5"/>
       <c r="M29" s="5"/>
       <c r="N29" s="5" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="O29" s="5" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="P29" s="15" t="n">
         <v>0.1</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="R29" s="14"/>
       <c r="S29" s="5" t="s">
         <v>57</v>
       </c>
       <c r="T29" s="5" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="U29" s="5" t="s">
         <v>59</v>
@@ -3736,7 +3766,7 @@
       <c r="Z29" s="5"/>
       <c r="AA29" s="5"/>
       <c r="AB29" s="5" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="AC29" s="5"/>
       <c r="AD29" s="5"/>
@@ -3748,7 +3778,7 @@
       <c r="AJ29" s="5"/>
       <c r="AK29" s="5"/>
       <c r="AL29" s="5" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="AM29" s="5"/>
       <c r="AN29" s="5"/>
@@ -3764,7 +3794,7 @@
         <v>43</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>45</v>
@@ -3775,17 +3805,17 @@
       <c r="F30" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="G30" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="H30" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="I30" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="J30" s="6" t="s">
+      <c r="G30" s="5" t="s">
         <v>127</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="J30" s="5" t="s">
+        <v>130</v>
       </c>
       <c r="K30" s="5" t="n">
         <v>29</v>
@@ -3793,10 +3823,10 @@
       <c r="L30" s="5"/>
       <c r="M30" s="5"/>
       <c r="N30" s="5" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="O30" s="5" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="P30" s="15" t="n">
         <v>0.1</v>
@@ -3809,7 +3839,7 @@
         <v>57</v>
       </c>
       <c r="T30" s="5" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="U30" s="5" t="s">
         <v>59</v>
@@ -3823,27 +3853,27 @@
       <c r="Z30" s="5"/>
       <c r="AA30" s="5"/>
       <c r="AB30" s="5" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="AC30" s="5" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="AD30" s="5" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="AE30" s="5"/>
       <c r="AF30" s="5"/>
       <c r="AG30" s="5" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="AH30" s="5"/>
       <c r="AI30" s="5"/>
       <c r="AJ30" s="5"/>
       <c r="AK30" s="5" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="AL30" s="1" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="AM30" s="5"/>
       <c r="AN30" s="5"/>
@@ -3859,7 +3889,7 @@
         <v>43</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>45</v>
@@ -3870,17 +3900,17 @@
       <c r="F31" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="G31" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="H31" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="I31" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="J31" s="6" t="s">
+      <c r="G31" s="5" t="s">
         <v>127</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>130</v>
       </c>
       <c r="K31" s="5" t="n">
         <v>30</v>
@@ -3888,10 +3918,10 @@
       <c r="L31" s="5"/>
       <c r="M31" s="5"/>
       <c r="N31" s="5" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="O31" s="5" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="P31" s="15" t="n">
         <v>0.1</v>
@@ -3904,7 +3934,7 @@
         <v>57</v>
       </c>
       <c r="T31" s="5" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="U31" s="5" t="s">
         <v>59</v>
@@ -3918,27 +3948,27 @@
       <c r="Z31" s="5"/>
       <c r="AA31" s="5"/>
       <c r="AB31" s="5" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="AC31" s="5" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="AD31" s="5" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="AE31" s="5"/>
       <c r="AF31" s="5"/>
       <c r="AG31" s="5" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="AH31" s="5"/>
       <c r="AI31" s="5"/>
       <c r="AJ31" s="5"/>
       <c r="AK31" s="5" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="AL31" s="5" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="AM31" s="5"/>
       <c r="AN31" s="5"/>
@@ -3954,7 +3984,7 @@
         <v>43</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>45</v>
@@ -3965,44 +3995,44 @@
       <c r="F32" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="G32" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="H32" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="I32" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="J32" s="6" t="s">
+      <c r="G32" s="5" t="s">
         <v>148</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="J32" s="5" t="s">
+        <v>151</v>
       </c>
       <c r="K32" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="L32" s="7" t="s">
-        <v>149</v>
+      <c r="L32" s="6" t="s">
+        <v>152</v>
       </c>
       <c r="M32" s="5"/>
       <c r="N32" s="5" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="O32" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="P32" s="10" t="n">
+        <v>154</v>
+      </c>
+      <c r="P32" s="9" t="n">
         <v>0.08</v>
       </c>
       <c r="Q32" s="5" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="R32" s="5"/>
       <c r="S32" s="5" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="T32" s="5"/>
       <c r="U32" s="5" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="V32" s="5"/>
       <c r="W32" s="5"/>
@@ -4010,13 +4040,13 @@
       <c r="Y32" s="5"/>
       <c r="Z32" s="5"/>
       <c r="AA32" s="5"/>
-      <c r="AB32" s="8"/>
+      <c r="AB32" s="7"/>
       <c r="AC32" s="5"/>
       <c r="AD32" s="5"/>
       <c r="AE32" s="5"/>
-      <c r="AF32" s="8"/>
-      <c r="AG32" s="8"/>
-      <c r="AH32" s="8"/>
+      <c r="AF32" s="7"/>
+      <c r="AG32" s="7"/>
+      <c r="AH32" s="7"/>
       <c r="AI32" s="5"/>
       <c r="AJ32" s="5"/>
       <c r="AK32" s="5"/>
@@ -4026,7 +4056,7 @@
       <c r="AO32" s="5"/>
       <c r="AP32" s="5"/>
       <c r="AQ32" s="5" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="27.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4037,7 +4067,7 @@
         <v>43</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>45</v>
@@ -4048,17 +4078,17 @@
       <c r="F33" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G33" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="H33" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="I33" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="J33" s="6" t="s">
+      <c r="G33" s="5" t="s">
         <v>148</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="J33" s="5" t="s">
+        <v>151</v>
       </c>
       <c r="K33" s="5" t="n">
         <v>32</v>
@@ -4068,16 +4098,16 @@
         <v>31</v>
       </c>
       <c r="N33" s="5" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="O33" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="P33" s="10" t="n">
+        <v>160</v>
+      </c>
+      <c r="P33" s="9" t="n">
         <v>0</v>
       </c>
       <c r="Q33" s="5" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="R33" s="5"/>
       <c r="S33" s="5"/>
@@ -4093,19 +4123,19 @@
       <c r="Y33" s="5"/>
       <c r="Z33" s="5"/>
       <c r="AA33" s="5"/>
-      <c r="AB33" s="8"/>
+      <c r="AB33" s="7"/>
       <c r="AC33" s="5" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="AD33" s="5"/>
       <c r="AE33" s="5"/>
-      <c r="AF33" s="8"/>
-      <c r="AG33" s="8"/>
-      <c r="AH33" s="8"/>
+      <c r="AF33" s="7"/>
+      <c r="AG33" s="7"/>
+      <c r="AH33" s="7"/>
       <c r="AI33" s="5"/>
       <c r="AJ33" s="5"/>
       <c r="AK33" s="5" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="AL33" s="5"/>
       <c r="AM33" s="5"/>
@@ -4113,7 +4143,7 @@
       <c r="AO33" s="5"/>
       <c r="AP33" s="5"/>
       <c r="AQ33" s="5" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="27.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4124,7 +4154,7 @@
         <v>43</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>45</v>
@@ -4135,17 +4165,17 @@
       <c r="F34" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G34" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="H34" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="I34" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="J34" s="6" t="s">
+      <c r="G34" s="5" t="s">
         <v>148</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="J34" s="5" t="s">
+        <v>151</v>
       </c>
       <c r="K34" s="5" t="n">
         <v>33</v>
@@ -4155,21 +4185,21 @@
         <v>31</v>
       </c>
       <c r="N34" s="5" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="O34" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="P34" s="10" t="n">
+        <v>165</v>
+      </c>
+      <c r="P34" s="9" t="n">
         <v>0</v>
       </c>
       <c r="Q34" s="5" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="R34" s="5"/>
       <c r="S34" s="5"/>
       <c r="T34" s="5" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="U34" s="5" t="s">
         <v>59</v>
@@ -4182,19 +4212,19 @@
       <c r="Y34" s="5"/>
       <c r="Z34" s="5"/>
       <c r="AA34" s="5"/>
-      <c r="AB34" s="8"/>
+      <c r="AB34" s="7"/>
       <c r="AC34" s="5" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="AD34" s="5"/>
       <c r="AE34" s="5"/>
-      <c r="AF34" s="8"/>
-      <c r="AG34" s="8"/>
-      <c r="AH34" s="8"/>
+      <c r="AF34" s="7"/>
+      <c r="AG34" s="7"/>
+      <c r="AH34" s="7"/>
       <c r="AI34" s="5"/>
       <c r="AJ34" s="5"/>
       <c r="AK34" s="5" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="AL34" s="5"/>
       <c r="AM34" s="5"/>
@@ -4211,7 +4241,7 @@
         <v>43</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>45</v>
@@ -4222,17 +4252,17 @@
       <c r="F35" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="G35" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="H35" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="I35" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="J35" s="6" t="s">
-        <v>167</v>
+      <c r="G35" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>170</v>
       </c>
       <c r="K35" s="5" t="n">
         <v>34</v>
@@ -4240,21 +4270,21 @@
       <c r="L35" s="5"/>
       <c r="M35" s="16"/>
       <c r="N35" s="5" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="O35" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="P35" s="10" t="n">
+        <v>172</v>
+      </c>
+      <c r="P35" s="9" t="n">
         <v>0.04</v>
       </c>
       <c r="Q35" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="R35" s="14"/>
       <c r="S35" s="5"/>
       <c r="T35" s="5" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="U35" s="5" t="s">
         <v>59</v>
@@ -4267,29 +4297,31 @@
       <c r="Y35" s="5"/>
       <c r="Z35" s="5"/>
       <c r="AA35" s="5" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="AB35" s="5" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="AC35" s="5"/>
       <c r="AD35" s="5"/>
       <c r="AE35" s="5"/>
-      <c r="AF35" s="8"/>
-      <c r="AG35" s="8"/>
-      <c r="AH35" s="8"/>
+      <c r="AF35" s="7"/>
+      <c r="AG35" s="7"/>
+      <c r="AH35" s="7"/>
+      <c r="AI35" s="0"/>
       <c r="AJ35" s="5"/>
       <c r="AK35" s="5" t="s">
         <v>60</v>
       </c>
       <c r="AL35" s="5" t="s">
-        <v>170</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="AM35" s="0"/>
       <c r="AN35" s="5"/>
       <c r="AO35" s="5"/>
       <c r="AP35" s="5"/>
       <c r="AQ35" s="5" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="27.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4300,7 +4332,7 @@
         <v>43</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>45</v>
@@ -4311,17 +4343,17 @@
       <c r="F36" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="G36" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="H36" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="I36" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="J36" s="6" t="s">
-        <v>167</v>
+      <c r="G36" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>170</v>
       </c>
       <c r="K36" s="5" t="n">
         <v>35</v>
@@ -4329,24 +4361,24 @@
       <c r="L36" s="5"/>
       <c r="M36" s="16"/>
       <c r="N36" s="5" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="O36" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="P36" s="10" t="n">
+        <v>176</v>
+      </c>
+      <c r="P36" s="9" t="n">
         <v>0.04</v>
       </c>
       <c r="Q36" s="5" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="R36" s="5"/>
       <c r="S36" s="5"/>
       <c r="T36" s="5" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="U36" s="5" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="V36" s="5"/>
       <c r="W36" s="5"/>
@@ -4356,21 +4388,21 @@
       <c r="Y36" s="5"/>
       <c r="Z36" s="5"/>
       <c r="AA36" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="AB36" s="8"/>
+        <v>159</v>
+      </c>
+      <c r="AB36" s="7"/>
       <c r="AC36" s="5" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="AD36" s="5"/>
       <c r="AE36" s="5"/>
-      <c r="AF36" s="8"/>
-      <c r="AG36" s="8"/>
-      <c r="AH36" s="8"/>
+      <c r="AF36" s="7"/>
+      <c r="AG36" s="7"/>
+      <c r="AH36" s="7"/>
       <c r="AI36" s="5"/>
       <c r="AJ36" s="5"/>
       <c r="AK36" s="5" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="AL36" s="5"/>
       <c r="AM36" s="5"/>
@@ -4378,7 +4410,7 @@
       <c r="AO36" s="5"/>
       <c r="AP36" s="5"/>
       <c r="AQ36" s="5" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="27.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4389,7 +4421,7 @@
         <v>43</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>45</v>
@@ -4400,17 +4432,17 @@
       <c r="F37" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="G37" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="H37" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="I37" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="J37" s="6" t="s">
-        <v>167</v>
+      <c r="G37" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>170</v>
       </c>
       <c r="K37" s="5" t="n">
         <v>36</v>
@@ -4418,22 +4450,22 @@
       <c r="L37" s="5"/>
       <c r="M37" s="16"/>
       <c r="N37" s="5" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="O37" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="P37" s="10" t="n">
+        <v>180</v>
+      </c>
+      <c r="P37" s="9" t="n">
         <v>0.04</v>
       </c>
       <c r="Q37" s="5" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="R37" s="5"/>
       <c r="S37" s="5"/>
       <c r="T37" s="5"/>
       <c r="U37" s="5" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="V37" s="5"/>
       <c r="W37" s="5"/>
@@ -4445,21 +4477,21 @@
         <v>19</v>
       </c>
       <c r="AA37" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="AB37" s="8"/>
+        <v>159</v>
+      </c>
+      <c r="AB37" s="7"/>
       <c r="AC37" s="5" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="AD37" s="5"/>
       <c r="AE37" s="5"/>
-      <c r="AF37" s="8"/>
-      <c r="AG37" s="8"/>
-      <c r="AH37" s="8"/>
+      <c r="AF37" s="7"/>
+      <c r="AG37" s="7"/>
+      <c r="AH37" s="7"/>
       <c r="AI37" s="5"/>
       <c r="AJ37" s="5"/>
       <c r="AK37" s="5" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="AL37" s="5"/>
       <c r="AM37" s="5"/>
@@ -4467,7 +4499,7 @@
       <c r="AO37" s="5"/>
       <c r="AP37" s="5"/>
       <c r="AQ37" s="5" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="27.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4478,7 +4510,7 @@
         <v>43</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>45</v>
@@ -4489,40 +4521,40 @@
       <c r="F38" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="G38" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="H38" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="I38" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="J38" s="6" t="s">
-        <v>181</v>
+      <c r="G38" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>184</v>
       </c>
       <c r="K38" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="L38" s="7" t="s">
-        <v>182</v>
+      <c r="L38" s="6" t="s">
+        <v>185</v>
       </c>
       <c r="M38" s="5"/>
       <c r="N38" s="5" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="O38" s="5" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="P38" s="15" t="n">
         <v>0.1</v>
       </c>
       <c r="Q38" s="5" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="R38" s="5"/>
       <c r="S38" s="5" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="T38" s="5"/>
       <c r="U38" s="5" t="s">
@@ -4546,10 +4578,10 @@
       <c r="AI38" s="5"/>
       <c r="AJ38" s="5"/>
       <c r="AK38" s="5" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="AL38" s="5" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="AM38" s="5"/>
       <c r="AN38" s="5"/>
@@ -4565,7 +4597,7 @@
         <v>43</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>45</v>
@@ -4576,17 +4608,17 @@
       <c r="F39" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G39" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="H39" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="I39" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="J39" s="6" t="s">
-        <v>181</v>
+      <c r="G39" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="J39" s="5" t="s">
+        <v>184</v>
       </c>
       <c r="K39" s="5" t="n">
         <v>38</v>
@@ -4596,10 +4628,10 @@
         <v>37</v>
       </c>
       <c r="N39" s="5" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="O39" s="5" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="P39" s="15" t="n">
         <v>0</v>
@@ -4626,10 +4658,10 @@
       <c r="Z39" s="5"/>
       <c r="AA39" s="5"/>
       <c r="AB39" s="5" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="AC39" s="5" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="AD39" s="5"/>
       <c r="AE39" s="5"/>
@@ -4639,10 +4671,10 @@
       <c r="AI39" s="5"/>
       <c r="AJ39" s="5"/>
       <c r="AK39" s="5" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="AL39" s="5" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="AM39" s="5"/>
       <c r="AN39" s="5"/>
@@ -4658,7 +4690,7 @@
         <v>43</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>45</v>
@@ -4669,17 +4701,17 @@
       <c r="F40" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G40" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="H40" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="I40" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="J40" s="6" t="s">
-        <v>181</v>
+      <c r="G40" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="J40" s="5" t="s">
+        <v>184</v>
       </c>
       <c r="K40" s="5" t="n">
         <v>39</v>
@@ -4689,10 +4721,10 @@
         <v>37</v>
       </c>
       <c r="N40" s="5" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="O40" s="5" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="P40" s="15" t="n">
         <v>0</v>
@@ -4722,7 +4754,7 @@
         <v>5000034</v>
       </c>
       <c r="AC40" s="5" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="AD40" s="5"/>
       <c r="AE40" s="5"/>
@@ -4732,17 +4764,17 @@
       <c r="AI40" s="5"/>
       <c r="AJ40" s="5"/>
       <c r="AK40" s="5" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="AL40" s="5" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="AM40" s="5"/>
       <c r="AN40" s="5"/>
       <c r="AO40" s="5"/>
       <c r="AP40" s="5"/>
       <c r="AQ40" s="5" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="27.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4753,13 +4785,13 @@
         <v>43</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>45</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
@@ -4769,28 +4801,28 @@
       <c r="K41" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="L41" s="7" t="s">
-        <v>198</v>
+      <c r="L41" s="6" t="s">
+        <v>201</v>
       </c>
       <c r="M41" s="5"/>
       <c r="N41" s="16" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="O41" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="P41" s="10" t="n">
+        <v>203</v>
+      </c>
+      <c r="P41" s="9" t="n">
         <v>0</v>
       </c>
       <c r="Q41" s="5" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="R41" s="5" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="S41" s="5"/>
       <c r="T41" s="5" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="U41" s="5"/>
       <c r="V41" s="5"/>
@@ -4824,13 +4856,13 @@
         <v>43</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>45</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
@@ -4845,23 +4877,23 @@
       </c>
       <c r="M42" s="5"/>
       <c r="N42" s="16" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="O42" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="P42" s="10" t="n">
+        <v>208</v>
+      </c>
+      <c r="P42" s="9" t="n">
         <v>0</v>
       </c>
       <c r="Q42" s="5" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="R42" s="5" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="S42" s="5"/>
       <c r="T42" s="5" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="U42" s="5"/>
       <c r="V42" s="5"/>
@@ -4870,8 +4902,8 @@
       <c r="Y42" s="5"/>
       <c r="Z42" s="5"/>
       <c r="AA42" s="5"/>
-      <c r="AB42" s="7" t="s">
-        <v>208</v>
+      <c r="AB42" s="6" t="s">
+        <v>211</v>
       </c>
       <c r="AC42" s="5"/>
       <c r="AD42" s="5"/>
@@ -4897,13 +4929,13 @@
         <v>43</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>45</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
@@ -4918,23 +4950,23 @@
       </c>
       <c r="M43" s="5"/>
       <c r="N43" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="O43" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="P43" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q43" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="O43" s="5" t="s">
+      <c r="R43" s="5" t="s">
         <v>210</v>
-      </c>
-      <c r="P43" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q43" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="R43" s="5" t="s">
-        <v>207</v>
       </c>
       <c r="S43" s="5"/>
       <c r="T43" s="5" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="U43" s="5"/>
       <c r="V43" s="5"/>
@@ -4943,8 +4975,8 @@
       <c r="Y43" s="5"/>
       <c r="Z43" s="5"/>
       <c r="AA43" s="5"/>
-      <c r="AB43" s="7" t="s">
-        <v>211</v>
+      <c r="AB43" s="6" t="s">
+        <v>214</v>
       </c>
       <c r="AC43" s="5"/>
       <c r="AD43" s="5"/>
@@ -4970,13 +5002,13 @@
         <v>43</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D44" s="5" t="s">
         <v>45</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
@@ -4991,23 +5023,23 @@
       </c>
       <c r="M44" s="5"/>
       <c r="N44" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="O44" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="P44" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q44" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="O44" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="P44" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q44" s="5" t="s">
-        <v>206</v>
-      </c>
       <c r="R44" s="5" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="S44" s="5"/>
       <c r="T44" s="5" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="U44" s="5"/>
       <c r="V44" s="5"/>
@@ -5016,8 +5048,8 @@
       <c r="Y44" s="5"/>
       <c r="Z44" s="5"/>
       <c r="AA44" s="5"/>
-      <c r="AB44" s="7" t="s">
-        <v>213</v>
+      <c r="AB44" s="6" t="s">
+        <v>216</v>
       </c>
       <c r="AC44" s="5"/>
       <c r="AD44" s="5"/>
@@ -5043,13 +5075,13 @@
         <v>43</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>45</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
@@ -5064,23 +5096,23 @@
       </c>
       <c r="M45" s="5"/>
       <c r="N45" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="O45" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="P45" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q45" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="O45" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="P45" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q45" s="5" t="s">
-        <v>206</v>
-      </c>
       <c r="R45" s="5" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="S45" s="5"/>
       <c r="T45" s="5" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="U45" s="5"/>
       <c r="V45" s="5"/>
@@ -5089,8 +5121,8 @@
       <c r="Y45" s="5"/>
       <c r="Z45" s="5"/>
       <c r="AA45" s="5"/>
-      <c r="AB45" s="7" t="s">
-        <v>215</v>
+      <c r="AB45" s="6" t="s">
+        <v>218</v>
       </c>
       <c r="AC45" s="5"/>
       <c r="AD45" s="5"/>
@@ -5109,7 +5141,7 @@
       <c r="AQ45" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AQ45"/>
+  <autoFilter ref="A1:AQ41"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -5134,17 +5166,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.63967611336032"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.74898785425101"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="180" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="17" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="180" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="17" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -5171,7 +5203,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.63967611336032"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.74898785425101"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5194,10 +5226,10 @@
         <v>28</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="I1" s="19" t="s">
         <v>42</v>
@@ -5206,18 +5238,18 @@
         <v>15</v>
       </c>
       <c r="K1" s="19" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="L1" s="19" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="M1" s="19" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="20" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>